<commit_message>
ajout de la dernière version de l'input bd9cc03614913b87ec5634cad1c830a43d4fb6ec
</commit_message>
<xml_diff>
--- a/update-input/ig/StructureDefinition-Medical-liability-unit.xlsx
+++ b/update-input/ig/StructureDefinition-Medical-liability-unit.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://ltsi.univ-rennes.fr/StructureDefinition/Medical-liability-unit</t>
+    <t>http://ltsi.univ-rennes.fr/StructureDefinition/MedicalLiabilityUnit</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-25T09:27:05+00:00</t>
+    <t>2024-03-25T09:30:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>